<commit_message>
funciona todo menos buzzer
</commit_message>
<xml_diff>
--- a/Conversiones ADC temp.xlsx
+++ b/Conversiones ADC temp.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a2108\Documents\GitHub\ESP32_4_sensores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EF2529-D94E-4BF7-AF48-D1CA99CF1460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFA306D-F983-43B4-BB91-E39BC3A0381B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{28D00C3E-F339-4CE3-AA76-D061D53DEB0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Pt100" sheetId="3" r:id="rId1"/>
-    <sheet name="PTC" sheetId="4" r:id="rId2"/>
+    <sheet name="Pt100 (2)" sheetId="6" r:id="rId2"/>
+    <sheet name="PTC" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="11">
   <si>
     <t>Temperatura</t>
   </si>
@@ -653,6 +654,1157 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.7712160979877508E-3"/>
+                  <c:y val="-0.26766987459900848"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Pt100'!$A$22:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Pt100'!$D$22:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.3933649289099526</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9266587677725113</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4599526066350665</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99324644549762864</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.52893364928909803</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.4620853080567559E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1AA6-49C7-B180-EB7F62EA1CBF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1049566016"/>
+        <c:axId val="1049566848"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1049566016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1049566848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1049566848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1049566016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Curva de calibracion</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.4745830865849292E-3"/>
+                  <c:y val="-0.19194558533209286"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Pt100 (2)'!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18653779179329133</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.37473233404710893</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.56411680761605476</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.75470068657131728</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.94649355144185232</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1399921977720302</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.335212055994943</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5311869962723543</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.7293997965412007</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.9288827623697979</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Pt100 (2)'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-89FC-4E31-BF32-F838E7629D52}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="430773904"/>
+        <c:axId val="430769968"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="430773904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="430769968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="430769968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="430773904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.7712160979877508E-3"/>
+                  <c:y val="-0.26766987459900848"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Pt100 (2)'!$A$22:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Pt100 (2)'!$D$22:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.3933649289099526</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9266587677725113</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4599526066350665</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99324644549762864</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.52893364928909803</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.4620853080567559E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F87A-4629-AB4A-2BFAAE4EAE73}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1049566016"/>
+        <c:axId val="1049566848"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1049566016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1049566848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1049566848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1049566016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -1086,6 +2238,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2118,20 +3390,1568 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1320165</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>39052</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>168592</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>527685</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>115252</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>725805</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>39052</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2158,10 +4978,127 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B6FBC9A-121D-6A7A-B6BF-41CB96C66881}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>168592</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>725805</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>39052</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76D04A8E-5045-468D-8600-A2139FDCF624}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25AF8567-EF6E-4049-BE44-793CE08939A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2501,10 +5438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0C69B2-9461-4A17-A229-4AA5AC131A0C}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2611,7 +5548,7 @@
         <v>88.22</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C4:C12" si="1">$G$4*($G$3/($G$2+$G$3)-B5/($G$2+B5))*1000</f>
+        <f t="shared" ref="C5:C12" si="1">$G$4*($G$3/($G$2+$G$3)-B5/($G$2+B5))*1000</f>
         <v>26.862705124574038</v>
       </c>
       <c r="D5">
@@ -2753,6 +5690,170 @@
       </c>
       <c r="C14" s="4">
         <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>100</v>
+      </c>
+      <c r="C22">
+        <f>$G$24*($G$23/($G$22+$G$23)-B22/($G$22+$G$23))*1000</f>
+        <v>23.696682464454977</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ref="D22:D27" si="2">C22*$C$31/1000</f>
+        <v>2.3933649289099526</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <v>2000</v>
+      </c>
+      <c r="H22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>101.95</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:C27" si="3">$G$24*($G$23/($G$22+$G$23)-B23/($G$22+$G$23))*1000</f>
+        <v>19.075829383886251</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>1.9266587677725113</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23">
+        <v>110</v>
+      </c>
+      <c r="H23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <v>103.9</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="3"/>
+        <v>14.454976303317491</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>1.4599526066350665</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="H24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="B25">
+        <v>105.85</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="3"/>
+        <v>9.8341232227487989</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>0.99324644549762864</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>20</v>
+      </c>
+      <c r="B26">
+        <v>107.79</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="3"/>
+        <v>5.2369668246445356</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>0.52893364928909803</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>109.73</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="3"/>
+        <v>0.63981042654027287</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>6.4620853080567559E-2</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F28" s="6">
+        <f>FORECAST(25,A22:A27,D22:D27)</f>
+        <v>-242.66624342271177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="3">
+        <f>100000/(C31-1)</f>
+        <v>1000</v>
+      </c>
+      <c r="C31" s="4">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2763,10 +5864,437 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED45066F-412C-4FD9-BB89-4B7458E0755F}">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <f>$G$4*($G$3/($G$2+$G$3)-B2/($G$2+$G$3))*1000</f>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>C2*$C$14/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>2000</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>-10</v>
+      </c>
+      <c r="B3">
+        <v>96.09</v>
+      </c>
+      <c r="C3">
+        <f>$G$4*($G$3/($G$2+$G$3)-B3/($G$2+B3))*1000</f>
+        <v>8.8827519901567289</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D12" si="0">C3*$C$14/1000</f>
+        <v>0.18653779179329133</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>-20</v>
+      </c>
+      <c r="B4">
+        <v>92.16</v>
+      </c>
+      <c r="C4">
+        <f>$G$4*($G$3/($G$2+$G$3)-B4/($G$2+B4))*1000</f>
+        <v>17.844396859386137</v>
+      </c>
+      <c r="D4">
+        <f>C4*$C$14/1000</f>
+        <v>0.37473233404710893</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>-30</v>
+      </c>
+      <c r="B5">
+        <v>88.22</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C12" si="1">$G$4*($G$3/($G$2+$G$3)-B5/($G$2+B5))*1000</f>
+        <v>26.862705124574038</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.56411680761605476</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>-40</v>
+      </c>
+      <c r="B6">
+        <v>84.27</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>35.938127931967493</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.75470068657131728</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>-50</v>
+      </c>
+      <c r="B7">
+        <v>80.31</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>45.071121497231061</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.94649355144185232</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>-60</v>
+      </c>
+      <c r="B8">
+        <v>76.33</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>54.285342751049065</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1.1399921977720302</v>
+      </c>
+      <c r="F8" s="6">
+        <f>FORECAST(2.4,A2:A12,D2:D12)</f>
+        <v>-124.98834113211747</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>-70</v>
+      </c>
+      <c r="B9">
+        <v>72.33</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>63.581526475949666</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1.335212055994943</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>-80</v>
+      </c>
+      <c r="B10">
+        <v>68.33</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>72.913666489159723</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1.5311869962723543</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>-90</v>
+      </c>
+      <c r="B11">
+        <v>64.3</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>82.352371263866701</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>1.7293997965412007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>-100</v>
+      </c>
+      <c r="B12">
+        <v>60.26</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>91.851560112847523</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1.9288827623697979</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="3">
+        <f>100000/(C14-1)</f>
+        <v>5000</v>
+      </c>
+      <c r="C14" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>100</v>
+      </c>
+      <c r="C22">
+        <f>$G$24*($G$23/($G$22+$G$23)-B22/($G$22+$G$23))*1000</f>
+        <v>23.696682464454977</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ref="D22:D27" si="2">C22*$C$31/1000</f>
+        <v>2.3933649289099526</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <v>2000</v>
+      </c>
+      <c r="H22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>101.95</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:C27" si="3">$G$24*($G$23/($G$22+$G$23)-B23/($G$22+$G$23))*1000</f>
+        <v>19.075829383886251</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>1.9266587677725113</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23">
+        <v>110</v>
+      </c>
+      <c r="H23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <v>103.9</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="3"/>
+        <v>14.454976303317491</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>1.4599526066350665</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="H24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="B25">
+        <v>105.85</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="3"/>
+        <v>9.8341232227487989</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>0.99324644549762864</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>20</v>
+      </c>
+      <c r="B26">
+        <v>107.79</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="3"/>
+        <v>5.2369668246445356</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>0.52893364928909803</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>109.73</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="3"/>
+        <v>0.63981042654027287</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>6.4620853080567559E-2</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F28" s="6">
+        <f>FORECAST(25,A22:A27,D22:D27)</f>
+        <v>-242.66624342271177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="3">
+        <f>100000/(C31-1)</f>
+        <v>1000</v>
+      </c>
+      <c r="C31" s="4">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{306305C3-D1BB-45B8-B859-F4BE86F42B29}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>

</xml_diff>